<commit_message>
se agregó el documento Consulta de criterios multiples
</commit_message>
<xml_diff>
--- a/00-Documentacion/Plan de Trabajo - Migracion.xlsx
+++ b/00-Documentacion/Plan de Trabajo - Migracion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\migracion\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2569F58-F2C2-4734-AC4A-A41C1F227010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D700F9-0EFB-4303-94FC-6DEF1B76C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" xr2:uid="{6819CE13-C260-433D-BD16-9098DCFB752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6819CE13-C260-433D-BD16-9098DCFB752F}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +380,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,6 +593,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1384,9 +1402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9614B30F-86D4-4947-8CA9-4AD146BFB102}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1420,7 @@
     <col min="9" max="9" width="21.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1470,7 +1488,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
@@ -1483,7 +1501,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
@@ -1496,7 +1514,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13" t="s">
@@ -1762,7 +1780,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="18" t="s">
         <v>2</v>
@@ -1775,7 +1793,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="18" t="s">
         <v>3</v>
@@ -1790,7 +1808,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
@@ -1803,7 +1821,7 @@
       <c r="H27" s="14"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="18"/>
       <c r="C28" s="20" t="s">
@@ -1849,7 +1867,7 @@
       </c>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="13"/>
       <c r="C30" s="20" t="s">
@@ -1880,7 +1898,7 @@
       <c r="H31" s="14"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="13" t="s">
         <v>23</v>
@@ -1893,7 +1911,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
       <c r="B33" s="18" t="s">
         <v>2</v>
@@ -1928,7 +1946,7 @@
       <c r="H35" s="14"/>
       <c r="I35" s="16"/>
     </row>
-    <row r="36" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
       <c r="B36" s="19" t="s">
         <v>16</v>
@@ -1943,7 +1961,7 @@
       <c r="H36" s="14"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="18" t="s">
         <v>2</v>
@@ -1964,7 +1982,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
       <c r="B38" s="18" t="s">
         <v>3</v>
@@ -1990,7 +2008,7 @@
       <c r="I38" s="16"/>
       <c r="J38" s="28"/>
     </row>
-    <row r="39" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
       <c r="B39" s="18"/>
       <c r="C39" s="20" t="s">
@@ -2013,7 +2031,7 @@
       </c>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
       <c r="B40" s="13"/>
       <c r="C40" s="20" t="s">
@@ -2037,7 +2055,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="28"/>
     </row>
-    <row r="41" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="21"/>
       <c r="C41" s="20" t="s">
@@ -2081,7 +2099,7 @@
       </c>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="21"/>
       <c r="C43" s="20" t="s">
@@ -2105,7 +2123,7 @@
       <c r="I43" s="16"/>
       <c r="J43" s="28"/>
     </row>
-    <row r="44" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="21"/>
       <c r="C44" s="20" t="s">
@@ -2129,7 +2147,7 @@
       <c r="I44" s="16"/>
       <c r="J44" s="29"/>
     </row>
-    <row r="45" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="21"/>
       <c r="C45" s="20" t="s">
@@ -2152,31 +2170,31 @@
       </c>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="21"/>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="34">
         <v>45425</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="34">
         <v>45432</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H46" s="34">
         <v>45432</v>
       </c>
-      <c r="I46" s="16"/>
+      <c r="I46" s="36"/>
       <c r="J46" s="28"/>
     </row>
-    <row r="47" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="21"/>
       <c r="C47" s="20" t="s">
@@ -2200,7 +2218,7 @@
       <c r="I47" s="16"/>
       <c r="J47" s="28"/>
     </row>
-    <row r="48" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="18"/>
       <c r="C48" s="30" t="s">
@@ -2224,7 +2242,7 @@
       <c r="I48" s="16"/>
       <c r="J48" s="28"/>
     </row>
-    <row r="49" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="B49" s="18"/>
       <c r="C49" s="20"/>
@@ -2235,7 +2253,7 @@
       <c r="H49" s="14"/>
       <c r="I49" s="16"/>
     </row>
-    <row r="50" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
       <c r="B50" s="18"/>
       <c r="C50" s="20"/>
@@ -2246,7 +2264,7 @@
       <c r="H50" s="14"/>
       <c r="I50" s="16"/>
     </row>
-    <row r="51" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A51" s="12"/>
       <c r="B51" s="18"/>
       <c r="C51" s="20"/>
@@ -2257,7 +2275,7 @@
       <c r="H51" s="14"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A52" s="12"/>
       <c r="B52" s="18"/>
       <c r="C52" s="20"/>
@@ -2268,7 +2286,7 @@
       <c r="H52" s="14"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A53" s="12"/>
       <c r="B53" s="18"/>
       <c r="C53" s="20"/>
@@ -2279,7 +2297,7 @@
       <c r="H53" s="14"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A54" s="12"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -2290,7 +2308,7 @@
       <c r="H54" s="14"/>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A55" s="22"/>
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
@@ -2301,7 +2319,7 @@
       <c r="H55" s="24"/>
       <c r="I55" s="25"/>
     </row>
-    <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="27" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>7</v>
       </c>
@@ -2343,7 +2361,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -2354,7 +2372,7 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A59" s="12"/>
       <c r="B59" s="13" t="s">
         <v>39</v>
@@ -2367,7 +2385,7 @@
       <c r="H59" s="15"/>
       <c r="I59" s="16"/>
     </row>
-    <row r="60" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
@@ -2380,7 +2398,7 @@
       <c r="H60" s="15"/>
       <c r="I60" s="16"/>
     </row>
-    <row r="61" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13" t="s">
@@ -2393,7 +2411,7 @@
       <c r="H61" s="14"/>
       <c r="I61" s="16"/>
     </row>
-    <row r="62" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A62" s="12"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -2404,7 +2422,7 @@
       <c r="H62" s="14"/>
       <c r="I62" s="16"/>
     </row>
-    <row r="63" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A63" s="12"/>
       <c r="B63" s="13" t="s">
         <v>40</v>
@@ -2417,7 +2435,7 @@
       <c r="H63" s="14"/>
       <c r="I63" s="16"/>
     </row>
-    <row r="64" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A64" s="12"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -2428,7 +2446,7 @@
       <c r="H64" s="14"/>
       <c r="I64" s="16"/>
     </row>
-    <row r="65" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A65" s="12"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -2439,7 +2457,7 @@
       <c r="H65" s="14"/>
       <c r="I65" s="16"/>
     </row>
-    <row r="66" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A66" s="12"/>
       <c r="B66" s="19" t="s">
         <v>76</v>
@@ -2452,7 +2470,7 @@
       <c r="H66" s="14"/>
       <c r="I66" s="16"/>
     </row>
-    <row r="67" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A67" s="12"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13" t="s">
@@ -2470,7 +2488,7 @@
       <c r="I67" s="16"/>
       <c r="J67" s="29"/>
     </row>
-    <row r="68" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A68" s="12"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -2481,7 +2499,7 @@
       <c r="H68" s="14"/>
       <c r="I68" s="16"/>
     </row>
-    <row r="69" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -2492,7 +2510,7 @@
       <c r="H69" s="14"/>
       <c r="I69" s="16"/>
     </row>
-    <row r="70" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A70" s="13"/>
       <c r="B70" s="13" t="s">
         <v>21</v>
@@ -2511,7 +2529,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A71" s="13"/>
       <c r="B71" s="13" t="s">
         <v>6</v>
@@ -2530,7 +2548,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -2541,7 +2559,7 @@
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
     </row>
-    <row r="73" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A73" s="13"/>
       <c r="B73" s="13" t="s">
         <v>56</v>
@@ -2554,7 +2572,7 @@
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
     </row>
-    <row r="74" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A74" s="13"/>
       <c r="B74" s="18" t="s">
         <v>2</v>
@@ -2571,7 +2589,7 @@
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
     </row>
-    <row r="75" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -2582,7 +2600,7 @@
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
     </row>
-    <row r="76" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -2593,7 +2611,7 @@
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>
     </row>
-    <row r="77" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -2604,7 +2622,7 @@
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
     </row>
-    <row r="78" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -2615,7 +2633,7 @@
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
     </row>
-    <row r="79" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -2626,7 +2644,7 @@
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
     </row>
-    <row r="80" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -2637,7 +2655,7 @@
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
     </row>
-    <row r="81" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -2648,7 +2666,7 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
     </row>
-    <row r="82" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -2659,7 +2677,7 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
     </row>
-    <row r="83" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -2670,7 +2688,7 @@
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
     </row>
-    <row r="84" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -2681,7 +2699,7 @@
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
     </row>
-    <row r="85" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -2692,7 +2710,7 @@
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
     </row>
-    <row r="86" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -2703,7 +2721,7 @@
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
     </row>
-    <row r="87" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -2714,7 +2732,7 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
     </row>
-    <row r="88" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -2725,7 +2743,7 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
     </row>
-    <row r="89" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -2736,7 +2754,7 @@
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
     </row>
-    <row r="90" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -2747,7 +2765,7 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
     </row>
-    <row r="91" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -2758,7 +2776,7 @@
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
     </row>
-    <row r="92" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -2769,7 +2787,7 @@
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
     </row>
-    <row r="93" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -2780,7 +2798,7 @@
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
     </row>
-    <row r="94" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -2791,7 +2809,7 @@
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
     </row>
-    <row r="95" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A95" s="23"/>
       <c r="B95" s="23"/>
       <c r="C95" s="23"/>
@@ -2815,7 +2833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A20D12-D618-4E4B-8EE3-A47A49335B77}">
   <dimension ref="B2:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se sube archivo de seguimiento
</commit_message>
<xml_diff>
--- a/00-Documentacion/Plan de Trabajo - Migracion.xlsx
+++ b/00-Documentacion/Plan de Trabajo - Migracion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\migracion\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_portal\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D700F9-0EFB-4303-94FC-6DEF1B76C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82902B80-D4AC-4AAB-B496-5E17C617AAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6819CE13-C260-433D-BD16-9098DCFB752F}"/>
   </bookViews>
@@ -21,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
   <si>
     <t>1 semana</t>
   </si>
@@ -307,6 +298,9 @@
   </si>
   <si>
     <t xml:space="preserve">Generacion de modelo para accesos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Módulo </t>
   </si>
 </sst>
 </file>
@@ -1402,9 +1396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9614B30F-86D4-4947-8CA9-4AD146BFB102}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1414,7 @@
     <col min="9" max="9" width="21.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -1488,7 +1482,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
@@ -1501,7 +1495,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13" t="s">
@@ -1514,7 +1508,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13" t="s">
@@ -1780,7 +1774,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="18" t="s">
         <v>2</v>
@@ -1793,7 +1787,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="18" t="s">
         <v>3</v>
@@ -1808,7 +1802,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13" t="s">
@@ -1821,7 +1815,7 @@
       <c r="H27" s="14"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="18"/>
       <c r="C28" s="20" t="s">
@@ -1867,7 +1861,7 @@
       </c>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="13"/>
       <c r="C30" s="20" t="s">
@@ -1898,7 +1892,7 @@
       <c r="H31" s="14"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="13" t="s">
         <v>23</v>
@@ -1911,7 +1905,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
       <c r="B33" s="18" t="s">
         <v>2</v>
@@ -1946,7 +1940,7 @@
       <c r="H35" s="14"/>
       <c r="I35" s="16"/>
     </row>
-    <row r="36" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="12"/>
       <c r="B36" s="19" t="s">
         <v>16</v>
@@ -1961,7 +1955,7 @@
       <c r="H36" s="14"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="18" t="s">
         <v>2</v>
@@ -1982,7 +1976,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
       <c r="B38" s="18" t="s">
         <v>3</v>
@@ -2008,7 +2002,7 @@
       <c r="I38" s="16"/>
       <c r="J38" s="28"/>
     </row>
-    <row r="39" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="12"/>
       <c r="B39" s="18"/>
       <c r="C39" s="20" t="s">
@@ -2031,7 +2025,7 @@
       </c>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
       <c r="B40" s="13"/>
       <c r="C40" s="20" t="s">
@@ -2055,7 +2049,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="28"/>
     </row>
-    <row r="41" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="12"/>
       <c r="B41" s="21"/>
       <c r="C41" s="20" t="s">
@@ -2099,7 +2093,7 @@
       </c>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="21"/>
       <c r="C43" s="20" t="s">
@@ -2123,7 +2117,7 @@
       <c r="I43" s="16"/>
       <c r="J43" s="28"/>
     </row>
-    <row r="44" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="21"/>
       <c r="C44" s="20" t="s">
@@ -2147,7 +2141,7 @@
       <c r="I44" s="16"/>
       <c r="J44" s="29"/>
     </row>
-    <row r="45" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
       <c r="B45" s="21"/>
       <c r="C45" s="20" t="s">
@@ -2177,7 +2171,7 @@
         <v>82</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E46" s="35" t="s">
         <v>83</v>
@@ -2194,14 +2188,14 @@
       <c r="I46" s="36"/>
       <c r="J46" s="28"/>
     </row>
-    <row r="47" spans="1:10" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="B47" s="21"/>
       <c r="C47" s="20" t="s">
         <v>38</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>67</v>
@@ -2218,14 +2212,14 @@
       <c r="I47" s="16"/>
       <c r="J47" s="28"/>
     </row>
-    <row r="48" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="18"/>
       <c r="C48" s="30" t="s">
         <v>86</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E48" s="32" t="s">
         <v>67</v>
@@ -2245,7 +2239,9 @@
     <row r="49" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="B49" s="18"/>
-      <c r="C49" s="20"/>
+      <c r="C49" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="D49" s="15"/>
       <c r="E49" s="14"/>
       <c r="F49" s="15"/>
@@ -2319,7 +2315,7 @@
       <c r="H55" s="24"/>
       <c r="I55" s="25"/>
     </row>
-    <row r="56" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>7</v>
       </c>
@@ -2385,7 +2381,7 @@
       <c r="H59" s="15"/>
       <c r="I59" s="16"/>
     </row>
-    <row r="60" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
@@ -2398,7 +2394,7 @@
       <c r="H60" s="15"/>
       <c r="I60" s="16"/>
     </row>
-    <row r="61" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13" t="s">
@@ -2499,7 +2495,7 @@
       <c r="H68" s="14"/>
       <c r="I68" s="16"/>
     </row>
-    <row r="69" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="12"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -2510,7 +2506,7 @@
       <c r="H69" s="14"/>
       <c r="I69" s="16"/>
     </row>
-    <row r="70" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="13"/>
       <c r="B70" s="13" t="s">
         <v>21</v>
@@ -2529,7 +2525,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="13"/>
       <c r="B71" s="13" t="s">
         <v>6</v>
@@ -2548,7 +2544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -2559,7 +2555,7 @@
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
     </row>
-    <row r="73" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="13"/>
       <c r="B73" s="13" t="s">
         <v>56</v>
@@ -2572,7 +2568,7 @@
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
     </row>
-    <row r="74" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="13"/>
       <c r="B74" s="18" t="s">
         <v>2</v>
@@ -2589,7 +2585,7 @@
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
     </row>
-    <row r="75" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -2600,7 +2596,7 @@
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
     </row>
-    <row r="76" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -2611,7 +2607,7 @@
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>
     </row>
-    <row r="77" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -2622,7 +2618,7 @@
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
     </row>
-    <row r="78" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -2633,7 +2629,7 @@
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
     </row>
-    <row r="79" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -2644,7 +2640,7 @@
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
     </row>
-    <row r="80" spans="1:10" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -2655,7 +2651,7 @@
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
     </row>
-    <row r="81" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -2666,7 +2662,7 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
     </row>
-    <row r="82" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -2677,7 +2673,7 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
     </row>
-    <row r="83" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -2688,7 +2684,7 @@
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
     </row>
-    <row r="84" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -2699,7 +2695,7 @@
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
     </row>
-    <row r="85" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -2710,7 +2706,7 @@
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
     </row>
-    <row r="86" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -2721,7 +2717,7 @@
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
     </row>
-    <row r="87" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -2732,7 +2728,7 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
     </row>
-    <row r="88" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -2743,7 +2739,7 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
     </row>
-    <row r="89" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -2754,7 +2750,7 @@
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
     </row>
-    <row r="90" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -2765,7 +2761,7 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
     </row>
-    <row r="91" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -2776,7 +2772,7 @@
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
     </row>
-    <row r="92" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -2787,7 +2783,7 @@
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
     </row>
-    <row r="93" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -2798,7 +2794,7 @@
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
     </row>
-    <row r="94" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -2809,7 +2805,7 @@
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
     </row>
-    <row r="95" spans="1:9" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="23"/>
       <c r="B95" s="23"/>
       <c r="C95" s="23"/>

</xml_diff>